<commit_message>
[SIT] Upgrade import saledata
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/import-employees.xlsx
+++ b/apps/core/fimport/static/fimport/template/import-employees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\MIS\misui\apps\core\fimport\static\fimport\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389EDEE9-996F-42CC-A59B-35776F628482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F88921-0B97-4C6F-8720-FF590A4B146C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Ngày tham gia</t>
   </si>
   <si>
-    <t>Người sinh</t>
-  </si>
-  <si>
     <t>Phòng ban</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
   </si>
 </sst>
 </file>
@@ -851,7 +851,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,48 +895,48 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -964,17 +964,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1015,7 +1015,7 @@
     </row>
     <row r="16" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -1024,23 +1024,23 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1048,10 +1048,10 @@
     </row>
     <row r="19" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="26" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -1098,95 +1098,95 @@
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="D27" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="E29" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E32" s="4"/>
     </row>

</xml_diff>

<commit_message>
[SIT][Import] Fix remark template import employee: DOB, Date Joined
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/import-employees.xlsx
+++ b/apps/core/fimport/static/fimport/template/import-employees.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\MIS\misui\apps\core\fimport\static\fimport\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F88921-0B97-4C6F-8720-FF590A4B146C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4584016-B7C5-400F-912D-C4E58CCB0D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
@@ -210,10 +210,6 @@
 - Ví dụ: EMP0001</t>
   </si>
   <si>
-    <t>- Định dạng ngày/tháng/năm (dd/mm/YYYY)
-- Ví dụ: 31/01/1970</t>
-  </si>
-  <si>
     <t>Lưu ý</t>
   </si>
   <si>
@@ -371,6 +367,10 @@
   </si>
   <si>
     <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>- Định dạng ngày-tháng-năm (dd-mm-YYYY)
+- Ví dụ: 31-01-1970</t>
   </si>
 </sst>
 </file>
@@ -851,25 +851,25 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="19.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="19.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="18" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="19.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,7 +895,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -904,7 +904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="146.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
@@ -927,10 +927,10 @@
         <v>45</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>46</v>
@@ -952,68 +952,68 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.88671875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="24.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>34</v>
       </c>
@@ -1022,7 +1022,7 @@
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
@@ -1032,10 +1032,10 @@
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
@@ -1057,7 +1057,7 @@
       <c r="D19" s="16"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
@@ -1068,26 +1068,26 @@
       <c r="D20" s="16"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25"/>
     </row>
-    <row r="26" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>42</v>
       </c>
@@ -1096,7 +1096,7 @@
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
     </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>12</v>
       </c>
@@ -1110,10 +1110,10 @@
         <v>16</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1142,10 +1142,10 @@
         <v>32</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>24</v>
       </c>
@@ -1190,42 +1190,42 @@
       </c>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>

</xml_diff>

<commit_message>
[Master] Hotfix import employee.
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/import-employees.xlsx
+++ b/apps/core/fimport/static/fimport/template/import-employees.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\MIS\misui\apps\core\fimport\static\fimport\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F88921-0B97-4C6F-8720-FF590A4B146C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4584016-B7C5-400F-912D-C4E58CCB0D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
@@ -210,10 +210,6 @@
 - Ví dụ: EMP0001</t>
   </si>
   <si>
-    <t>- Định dạng ngày/tháng/năm (dd/mm/YYYY)
-- Ví dụ: 31/01/1970</t>
-  </si>
-  <si>
     <t>Lưu ý</t>
   </si>
   <si>
@@ -371,6 +367,10 @@
   </si>
   <si>
     <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>- Định dạng ngày-tháng-năm (dd-mm-YYYY)
+- Ví dụ: 31-01-1970</t>
   </si>
 </sst>
 </file>
@@ -851,25 +851,25 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="19.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="19.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="18" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="19.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,7 +895,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -904,7 +904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="146.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
@@ -927,10 +927,10 @@
         <v>45</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>46</v>
@@ -952,68 +952,68 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.88671875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="24.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>34</v>
       </c>
@@ -1022,7 +1022,7 @@
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
@@ -1032,10 +1032,10 @@
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
@@ -1057,7 +1057,7 @@
       <c r="D19" s="16"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
@@ -1068,26 +1068,26 @@
       <c r="D20" s="16"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25"/>
     </row>
-    <row r="26" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>42</v>
       </c>
@@ -1096,7 +1096,7 @@
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
     </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>12</v>
       </c>
@@ -1110,10 +1110,10 @@
         <v>16</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1142,10 +1142,10 @@
         <v>32</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>24</v>
       </c>
@@ -1190,42 +1190,42 @@
       </c>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>

</xml_diff>